<commit_message>
Stacked Radial - for second part in data bucket
</commit_message>
<xml_diff>
--- a/mymap/jsons/GenderGap_Find4Hourglass.xlsx
+++ b/mymap/jsons/GenderGap_Find4Hourglass.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="0" windowWidth="27340" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="29860" windowHeight="16440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Total_W2E" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="184">
   <si>
     <t xml:space="preserve">Labour force participation                              </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -710,6 +710,18 @@
   <si>
     <t>Female-to-male ratio (0.00 = INEQUALITY 1.00 = EQUALITY)</t>
   </si>
+  <si>
+    <t>ECONOMIC PARTICIPATION AND OPPORTUNITY</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
 </sst>
 </file>
 
@@ -1119,7 +1131,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1261,8 +1273,70 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1553,6 +1627,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="108" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1638,7 +1718,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="203">
     <cellStyle name="Bad" xfId="107" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="108" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1709,6 +1789,37 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="106" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1778,6 +1889,37 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="105"/>
   </cellStyles>
@@ -2154,11 +2296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2143831784"/>
-        <c:axId val="-2143828104"/>
+        <c:axId val="-2139658376"/>
+        <c:axId val="-2143333032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143831784"/>
+        <c:axId val="-2139658376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,7 +2309,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143828104"/>
+        <c:crossAx val="-2143333032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2175,7 +2317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143828104"/>
+        <c:axId val="-2143333032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2333,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2143831784"/>
+        <c:crossAx val="-2139658376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2406,11 +2548,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143774072"/>
-        <c:axId val="-2143653016"/>
+        <c:axId val="-2143376408"/>
+        <c:axId val="-2143401960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143774072"/>
+        <c:axId val="-2143376408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,7 +2561,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143653016"/>
+        <c:crossAx val="-2143401960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2427,7 +2569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143653016"/>
+        <c:axId val="-2143401960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,7 +2580,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2143774072"/>
+        <c:crossAx val="-2143376408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2864,8 +3006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2894,37 +3036,37 @@
     <row r="1" spans="1:27" ht="34" customHeight="1">
       <c r="A1" s="97"/>
       <c r="B1" s="97"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="F1" s="115" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -2941,9 +3083,9 @@
     <row r="2" spans="1:27" ht="113" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -3012,13 +3154,13 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="105">
-        <v>1</v>
-      </c>
-      <c r="C3" s="108" t="s">
+      <c r="B3" s="107">
+        <v>1</v>
+      </c>
+      <c r="C3" s="110" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="92">
@@ -3086,9 +3228,9 @@
       </c>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="111"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="108"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="110"/>
       <c r="D4" s="92">
         <v>2010</v>
       </c>
@@ -3154,9 +3296,9 @@
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="111"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="110"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -3222,7 +3364,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="111"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="91"/>
       <c r="C6" s="92"/>
       <c r="D6" s="25"/>
@@ -3244,11 +3386,11 @@
       <c r="X6" s="101"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="111"/>
-      <c r="B7" s="105">
+      <c r="A7" s="113"/>
+      <c r="B7" s="107">
         <v>2</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="110" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="92">
@@ -3316,9 +3458,9 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="111"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="108"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="92">
         <v>2010</v>
       </c>
@@ -3384,9 +3526,9 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="111"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="108"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="110"/>
       <c r="D9" s="25">
         <v>2014</v>
       </c>
@@ -3452,7 +3594,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="111"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
       <c r="D10" s="25"/>
@@ -3474,11 +3616,11 @@
       <c r="X10" s="101"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="111"/>
-      <c r="B11" s="105">
+      <c r="A11" s="113"/>
+      <c r="B11" s="107">
         <v>3</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="110" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="92">
@@ -3546,9 +3688,9 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="111"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="108"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="110"/>
       <c r="D12" s="92">
         <v>2010</v>
       </c>
@@ -3614,9 +3756,9 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="111"/>
-      <c r="B13" s="107"/>
-      <c r="C13" s="108"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="25">
         <v>2014</v>
       </c>
@@ -3682,7 +3824,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="111"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92"/>
       <c r="D14" s="25"/>
@@ -3704,11 +3846,11 @@
       <c r="X14" s="101"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="111"/>
-      <c r="B15" s="105">
+      <c r="A15" s="113"/>
+      <c r="B15" s="107">
         <v>4</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="110" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="92">
@@ -3776,9 +3918,9 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="111"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="108"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="110"/>
       <c r="D16" s="92">
         <v>2010</v>
       </c>
@@ -3844,9 +3986,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="111"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -3912,7 +4054,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="111"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
       <c r="D18" s="25"/>
@@ -3934,11 +4076,11 @@
       <c r="X18" s="101"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A19" s="111"/>
-      <c r="B19" s="105">
+      <c r="A19" s="113"/>
+      <c r="B19" s="107">
         <v>5</v>
       </c>
-      <c r="C19" s="108" t="s">
+      <c r="C19" s="110" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="92">
@@ -4006,9 +4148,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="111"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="108"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="92">
         <v>2010</v>
       </c>
@@ -4074,9 +4216,9 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="111"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="108"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="110"/>
       <c r="D21" s="25">
         <v>2014</v>
       </c>
@@ -4142,7 +4284,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="111"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="91"/>
       <c r="C22" s="92"/>
       <c r="D22" s="25"/>
@@ -4164,11 +4306,11 @@
       <c r="X22" s="101"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="111"/>
-      <c r="B23" s="105">
+      <c r="A23" s="113"/>
+      <c r="B23" s="107">
         <v>6</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="110" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="92">
@@ -4236,9 +4378,9 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="111"/>
-      <c r="B24" s="106"/>
-      <c r="C24" s="108"/>
+      <c r="A24" s="113"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="110"/>
       <c r="D24" s="92">
         <v>2010</v>
       </c>
@@ -4304,9 +4446,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="111"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="108"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="110"/>
       <c r="D25" s="25">
         <v>2014</v>
       </c>
@@ -4372,7 +4514,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="111"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="91"/>
       <c r="C26" s="92"/>
       <c r="D26" s="25"/>
@@ -4394,11 +4536,11 @@
       <c r="X26" s="101"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="111"/>
-      <c r="B27" s="105">
+      <c r="A27" s="113"/>
+      <c r="B27" s="107">
         <v>7</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="110" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="92">
@@ -4466,9 +4608,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="111"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="108"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="110"/>
       <c r="D28" s="92">
         <v>2010</v>
       </c>
@@ -4534,9 +4676,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="111"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="108"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="110"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -4602,7 +4744,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="111"/>
+      <c r="A30" s="113"/>
       <c r="B30" s="91"/>
       <c r="C30" s="95"/>
       <c r="D30" s="25"/>
@@ -4624,11 +4766,11 @@
       <c r="X30" s="101"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="111"/>
-      <c r="B31" s="105">
+      <c r="A31" s="113"/>
+      <c r="B31" s="107">
         <v>8</v>
       </c>
-      <c r="C31" s="114" t="s">
+      <c r="C31" s="116" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="92">
@@ -4696,9 +4838,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="111"/>
-      <c r="B32" s="106"/>
-      <c r="C32" s="115"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="117"/>
       <c r="D32" s="92">
         <v>2010</v>
       </c>
@@ -4764,9 +4906,9 @@
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="111"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="116"/>
+      <c r="A33" s="113"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="25">
         <v>2014</v>
       </c>
@@ -4832,7 +4974,7 @@
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" s="111"/>
+      <c r="A34" s="113"/>
       <c r="B34" s="91"/>
       <c r="C34" s="96"/>
       <c r="D34" s="25"/>
@@ -4854,11 +4996,11 @@
       <c r="X34" s="101"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="111"/>
-      <c r="B35" s="105">
+      <c r="A35" s="113"/>
+      <c r="B35" s="107">
         <v>9</v>
       </c>
-      <c r="C35" s="108" t="s">
+      <c r="C35" s="110" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="92">
@@ -4926,9 +5068,9 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="111"/>
-      <c r="B36" s="106"/>
-      <c r="C36" s="108"/>
+      <c r="A36" s="113"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="110"/>
       <c r="D36" s="92">
         <v>2010</v>
       </c>
@@ -4994,9 +5136,9 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="111"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="108"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="110"/>
       <c r="D37" s="25">
         <v>2014</v>
       </c>
@@ -5062,7 +5204,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="111"/>
+      <c r="A38" s="113"/>
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="25"/>
@@ -5084,11 +5226,11 @@
       <c r="X38" s="101"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="111"/>
-      <c r="B39" s="105">
+      <c r="A39" s="113"/>
+      <c r="B39" s="107">
         <v>10</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="110" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="92">
@@ -5156,9 +5298,9 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="111"/>
-      <c r="B40" s="106"/>
-      <c r="C40" s="108"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="110"/>
       <c r="D40" s="92">
         <v>2010</v>
       </c>
@@ -5224,9 +5366,9 @@
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="111"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="108"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="110"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -5292,7 +5434,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="111"/>
+      <c r="A42" s="113"/>
       <c r="B42" s="91"/>
       <c r="C42" s="92"/>
       <c r="D42" s="25"/>
@@ -5314,11 +5456,11 @@
       <c r="X42" s="101"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="111"/>
-      <c r="B43" s="105">
+      <c r="A43" s="113"/>
+      <c r="B43" s="107">
         <v>11</v>
       </c>
-      <c r="C43" s="108" t="s">
+      <c r="C43" s="110" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="92">
@@ -5386,9 +5528,9 @@
       </c>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="111"/>
-      <c r="B44" s="106"/>
-      <c r="C44" s="108"/>
+      <c r="A44" s="113"/>
+      <c r="B44" s="108"/>
+      <c r="C44" s="110"/>
       <c r="D44" s="92">
         <v>2010</v>
       </c>
@@ -5454,9 +5596,9 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="111"/>
-      <c r="B45" s="107"/>
-      <c r="C45" s="108"/>
+      <c r="A45" s="113"/>
+      <c r="B45" s="109"/>
+      <c r="C45" s="110"/>
       <c r="D45" s="25">
         <v>2014</v>
       </c>
@@ -5522,7 +5664,7 @@
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="111"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="91"/>
       <c r="C46" s="92"/>
       <c r="D46" s="25"/>
@@ -5544,11 +5686,11 @@
       <c r="X46" s="101"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="111"/>
-      <c r="B47" s="105">
+      <c r="A47" s="113"/>
+      <c r="B47" s="107">
         <v>12</v>
       </c>
-      <c r="C47" s="108" t="s">
+      <c r="C47" s="110" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="92">
@@ -5616,9 +5758,9 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="111"/>
-      <c r="B48" s="106"/>
-      <c r="C48" s="108"/>
+      <c r="A48" s="113"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="110"/>
       <c r="D48" s="92">
         <v>2010</v>
       </c>
@@ -5684,9 +5826,9 @@
       </c>
     </row>
     <row r="49" spans="1:41">
-      <c r="A49" s="111"/>
-      <c r="B49" s="107"/>
-      <c r="C49" s="108"/>
+      <c r="A49" s="113"/>
+      <c r="B49" s="109"/>
+      <c r="C49" s="110"/>
       <c r="D49" s="25">
         <v>2014</v>
       </c>
@@ -5752,7 +5894,7 @@
       </c>
     </row>
     <row r="50" spans="1:41">
-      <c r="A50" s="111"/>
+      <c r="A50" s="113"/>
       <c r="B50" s="91"/>
       <c r="C50" s="92"/>
       <c r="D50" s="25"/>
@@ -5774,11 +5916,11 @@
       <c r="X50" s="101"/>
     </row>
     <row r="51" spans="1:41">
-      <c r="A51" s="111"/>
-      <c r="B51" s="105">
+      <c r="A51" s="113"/>
+      <c r="B51" s="107">
         <v>13</v>
       </c>
-      <c r="C51" s="108" t="s">
+      <c r="C51" s="110" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="92">
@@ -5846,9 +5988,9 @@
       </c>
     </row>
     <row r="52" spans="1:41">
-      <c r="A52" s="111"/>
-      <c r="B52" s="106"/>
-      <c r="C52" s="108"/>
+      <c r="A52" s="113"/>
+      <c r="B52" s="108"/>
+      <c r="C52" s="110"/>
       <c r="D52" s="92">
         <v>2010</v>
       </c>
@@ -5914,9 +6056,9 @@
       </c>
     </row>
     <row r="53" spans="1:41">
-      <c r="A53" s="111"/>
-      <c r="B53" s="107"/>
-      <c r="C53" s="108"/>
+      <c r="A53" s="113"/>
+      <c r="B53" s="109"/>
+      <c r="C53" s="110"/>
       <c r="D53" s="25">
         <v>2014</v>
       </c>
@@ -5982,79 +6124,79 @@
       </c>
     </row>
     <row r="54" spans="1:41">
-      <c r="A54" s="111"/>
+      <c r="A54" s="113"/>
     </row>
     <row r="55" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="111"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="86"/>
-      <c r="C55" s="120" t="s">
+      <c r="C55" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="120"/>
-      <c r="E55" s="120"/>
-      <c r="F55" s="120" t="s">
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="120"/>
-      <c r="H55" s="120"/>
-      <c r="I55" s="120" t="s">
+      <c r="G55" s="122"/>
+      <c r="H55" s="122"/>
+      <c r="I55" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="120"/>
-      <c r="K55" s="120"/>
-      <c r="L55" s="120" t="s">
+      <c r="J55" s="122"/>
+      <c r="K55" s="122"/>
+      <c r="L55" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="120"/>
-      <c r="N55" s="120"/>
-      <c r="O55" s="120" t="s">
+      <c r="M55" s="122"/>
+      <c r="N55" s="122"/>
+      <c r="O55" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="P55" s="120"/>
-      <c r="Q55" s="120"/>
-      <c r="R55" s="117" t="s">
+      <c r="P55" s="122"/>
+      <c r="Q55" s="122"/>
+      <c r="R55" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="118"/>
-      <c r="T55" s="119"/>
-      <c r="U55" s="120" t="s">
+      <c r="S55" s="120"/>
+      <c r="T55" s="121"/>
+      <c r="U55" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="120"/>
-      <c r="W55" s="120"/>
-      <c r="X55" s="117" t="s">
+      <c r="V55" s="122"/>
+      <c r="W55" s="122"/>
+      <c r="X55" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="118"/>
-      <c r="Z55" s="119"/>
-      <c r="AA55" s="120" t="s">
+      <c r="Y55" s="120"/>
+      <c r="Z55" s="121"/>
+      <c r="AA55" s="122" t="s">
         <v>105</v>
       </c>
-      <c r="AB55" s="120"/>
-      <c r="AC55" s="120"/>
-      <c r="AD55" s="120" t="s">
+      <c r="AB55" s="122"/>
+      <c r="AC55" s="122"/>
+      <c r="AD55" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="120"/>
-      <c r="AF55" s="120"/>
-      <c r="AG55" s="120" t="s">
+      <c r="AE55" s="122"/>
+      <c r="AF55" s="122"/>
+      <c r="AG55" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="AH55" s="120"/>
-      <c r="AI55" s="120"/>
-      <c r="AJ55" s="120" t="s">
+      <c r="AH55" s="122"/>
+      <c r="AI55" s="122"/>
+      <c r="AJ55" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="120"/>
-      <c r="AL55" s="120"/>
-      <c r="AM55" s="120" t="s">
+      <c r="AK55" s="122"/>
+      <c r="AL55" s="122"/>
+      <c r="AM55" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="AN55" s="120"/>
-      <c r="AO55" s="120"/>
+      <c r="AN55" s="122"/>
+      <c r="AO55" s="122"/>
     </row>
     <row r="56" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A56" s="112"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86" t="s">
         <v>72</v>
@@ -6295,10 +6437,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="123" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="122"/>
+      <c r="B58" s="124"/>
       <c r="C58" s="79">
         <v>2006</v>
       </c>
@@ -6335,10 +6477,10 @@
       <c r="Y58" s="100"/>
     </row>
     <row r="59" spans="1:41" ht="16" thickTop="1">
-      <c r="A59" s="123" t="s">
+      <c r="A59" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="123"/>
+      <c r="B59" s="125"/>
       <c r="C59">
         <f xml:space="preserve"> C57/115</f>
         <v>3.4782608695652174E-2</v>
@@ -6497,10 +6639,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="124" t="s">
+      <c r="A60" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="124"/>
+      <c r="B60" s="126"/>
       <c r="C60">
         <f xml:space="preserve"> C59*72</f>
         <v>2.5043478260869567</v>
@@ -6659,10 +6801,10 @@
       </c>
     </row>
     <row r="61" spans="1:41" s="80" customFormat="1">
-      <c r="A61" s="125" t="s">
+      <c r="A61" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="125"/>
+      <c r="B61" s="127"/>
       <c r="C61" s="80">
         <f xml:space="preserve"> 72-C60</f>
         <v>69.495652173913044</v>
@@ -6972,77 +7114,77 @@
       <c r="X66" s="85"/>
     </row>
     <row r="67" spans="1:41">
-      <c r="C67" s="120" t="s">
+      <c r="C67" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="120"/>
-      <c r="E67" s="120"/>
-      <c r="F67" s="117" t="s">
+      <c r="D67" s="122"/>
+      <c r="E67" s="122"/>
+      <c r="F67" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="118"/>
-      <c r="H67" s="119"/>
-      <c r="I67" s="120" t="s">
+      <c r="G67" s="120"/>
+      <c r="H67" s="121"/>
+      <c r="I67" s="122" t="s">
         <v>105</v>
       </c>
-      <c r="J67" s="120"/>
-      <c r="K67" s="120"/>
-      <c r="L67" s="120" t="s">
+      <c r="J67" s="122"/>
+      <c r="K67" s="122"/>
+      <c r="L67" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="M67" s="120"/>
-      <c r="N67" s="120"/>
-      <c r="O67" s="120" t="s">
+      <c r="M67" s="122"/>
+      <c r="N67" s="122"/>
+      <c r="O67" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="P67" s="120"/>
-      <c r="Q67" s="120"/>
-      <c r="R67" s="117" t="s">
+      <c r="P67" s="122"/>
+      <c r="Q67" s="122"/>
+      <c r="R67" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="S67" s="118"/>
-      <c r="T67" s="119"/>
-      <c r="U67" s="120" t="s">
+      <c r="S67" s="120"/>
+      <c r="T67" s="121"/>
+      <c r="U67" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="V67" s="120"/>
-      <c r="W67" s="120"/>
-      <c r="X67" s="120" t="s">
+      <c r="V67" s="122"/>
+      <c r="W67" s="122"/>
+      <c r="X67" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="Y67" s="120"/>
-      <c r="Z67" s="120"/>
-      <c r="AA67" s="120" t="s">
+      <c r="Y67" s="122"/>
+      <c r="Z67" s="122"/>
+      <c r="AA67" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="120"/>
-      <c r="AC67" s="120"/>
-      <c r="AD67" s="120" t="s">
+      <c r="AB67" s="122"/>
+      <c r="AC67" s="122"/>
+      <c r="AD67" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="AE67" s="120"/>
-      <c r="AF67" s="120"/>
-      <c r="AG67" s="120" t="s">
+      <c r="AE67" s="122"/>
+      <c r="AF67" s="122"/>
+      <c r="AG67" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AH67" s="120"/>
-      <c r="AI67" s="120"/>
-      <c r="AJ67" s="120" t="s">
+      <c r="AH67" s="122"/>
+      <c r="AI67" s="122"/>
+      <c r="AJ67" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="AK67" s="120"/>
-      <c r="AL67" s="120"/>
-      <c r="AM67" s="120" t="s">
+      <c r="AK67" s="122"/>
+      <c r="AL67" s="122"/>
+      <c r="AM67" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="AN67" s="120"/>
-      <c r="AO67" s="120"/>
+      <c r="AN67" s="122"/>
+      <c r="AO67" s="122"/>
     </row>
     <row r="68" spans="1:41" ht="70">
-      <c r="A68" s="126" t="s">
+      <c r="A68" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="127"/>
+      <c r="B68" s="129"/>
       <c r="C68" s="86" t="s">
         <v>99</v>
       </c>
@@ -7162,8 +7304,8 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="16" thickBot="1">
-      <c r="A69" s="128"/>
-      <c r="B69" s="129"/>
+      <c r="A69" s="130"/>
+      <c r="B69" s="131"/>
       <c r="C69" s="86">
         <v>23</v>
       </c>
@@ -7283,10 +7425,10 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="16" thickTop="1">
-      <c r="A70" s="123" t="s">
+      <c r="A70" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="123"/>
+      <c r="B70" s="125"/>
       <c r="C70">
         <f xml:space="preserve"> C69/115</f>
         <v>0.2</v>
@@ -7445,10 +7587,10 @@
       </c>
     </row>
     <row r="71" spans="1:41">
-      <c r="A71" s="124" t="s">
+      <c r="A71" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="124"/>
+      <c r="B71" s="126"/>
       <c r="C71">
         <f xml:space="preserve"> C70*65</f>
         <v>13</v>
@@ -7607,10 +7749,10 @@
       </c>
     </row>
     <row r="72" spans="1:41">
-      <c r="A72" s="125" t="s">
+      <c r="A72" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="125"/>
+      <c r="B72" s="127"/>
       <c r="C72" s="80">
         <f xml:space="preserve"> 65-C71</f>
         <v>52</v>
@@ -7860,7 +8002,7 @@
   <dimension ref="A1:AO70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F4" sqref="F4:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7886,37 +8028,37 @@
     <row r="1" spans="1:24" ht="34" customHeight="1">
       <c r="A1" s="57"/>
       <c r="B1" s="57"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -7929,16 +8071,16 @@
       <c r="W1" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="108" t="s">
+      <c r="X1" s="110" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="144">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -7993,16 +8135,16 @@
       <c r="W2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="108"/>
+      <c r="X2" s="110"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="105">
-        <v>1</v>
-      </c>
-      <c r="C3" s="108" t="s">
+      <c r="B3" s="107">
+        <v>1</v>
+      </c>
+      <c r="C3" s="110" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="54">
@@ -8070,9 +8212,9 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="111"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="108"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="110"/>
       <c r="D4" s="54">
         <v>2010</v>
       </c>
@@ -8138,9 +8280,9 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="111"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="110"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -8206,11 +8348,11 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1">
-      <c r="A6" s="111"/>
-      <c r="B6" s="105">
+      <c r="A6" s="113"/>
+      <c r="B6" s="107">
         <v>2</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="110" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="54">
@@ -8278,9 +8420,9 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="111"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="108"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="110"/>
       <c r="D7" s="54">
         <v>2010</v>
       </c>
@@ -8346,9 +8488,9 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="111"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -8414,11 +8556,11 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="111"/>
-      <c r="B9" s="105">
+      <c r="A9" s="113"/>
+      <c r="B9" s="107">
         <v>3</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="110" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="54">
@@ -8486,9 +8628,9 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="111"/>
-      <c r="B10" s="106"/>
-      <c r="C10" s="108"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="110"/>
       <c r="D10" s="54">
         <v>2010</v>
       </c>
@@ -8554,9 +8696,9 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="111"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="108"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -8622,11 +8764,11 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="111"/>
-      <c r="B12" s="105">
+      <c r="A12" s="113"/>
+      <c r="B12" s="107">
         <v>4</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="110" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="54">
@@ -8694,9 +8836,9 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="111"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="108"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="54">
         <v>2010</v>
       </c>
@@ -8762,9 +8904,9 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="111"/>
-      <c r="B14" s="107"/>
-      <c r="C14" s="108"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -8830,11 +8972,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A15" s="111"/>
-      <c r="B15" s="105">
+      <c r="A15" s="113"/>
+      <c r="B15" s="107">
         <v>5</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="110" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54">
@@ -8902,9 +9044,9 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="111"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="108"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="110"/>
       <c r="D16" s="54">
         <v>2010</v>
       </c>
@@ -8970,9 +9112,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="111"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -9038,11 +9180,11 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A18" s="111"/>
-      <c r="B18" s="105">
+      <c r="A18" s="113"/>
+      <c r="B18" s="107">
         <v>6</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="110" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="54">
@@ -9110,9 +9252,9 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="111"/>
-      <c r="B19" s="106"/>
-      <c r="C19" s="108"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="54">
         <v>2010</v>
       </c>
@@ -9178,9 +9320,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="111"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="108"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -9246,11 +9388,11 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="111"/>
-      <c r="B21" s="105">
+      <c r="A21" s="113"/>
+      <c r="B21" s="107">
         <v>7</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="110" t="s">
         <v>70</v>
       </c>
       <c r="D21" s="54">
@@ -9318,9 +9460,9 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="111"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="108"/>
+      <c r="A22" s="113"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="110"/>
       <c r="D22" s="54">
         <v>2010</v>
       </c>
@@ -9386,9 +9528,9 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="111"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
+      <c r="A23" s="113"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -9454,11 +9596,11 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="111"/>
-      <c r="B24" s="105">
+      <c r="A24" s="113"/>
+      <c r="B24" s="107">
         <v>8</v>
       </c>
-      <c r="C24" s="114" t="s">
+      <c r="C24" s="116" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="54">
@@ -9526,9 +9668,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="111"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="115"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="117"/>
       <c r="D25" s="54">
         <v>2010</v>
       </c>
@@ -9594,9 +9736,9 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="111"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="116"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="118"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -9662,11 +9804,11 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="111"/>
-      <c r="B27" s="105">
+      <c r="A27" s="113"/>
+      <c r="B27" s="107">
         <v>9</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="110" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="54">
@@ -9734,9 +9876,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="111"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="108"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="110"/>
       <c r="D28" s="54">
         <v>2010</v>
       </c>
@@ -9802,9 +9944,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="111"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="108"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="110"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -9870,11 +10012,11 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="111"/>
-      <c r="B30" s="105">
+      <c r="A30" s="113"/>
+      <c r="B30" s="107">
         <v>10</v>
       </c>
-      <c r="C30" s="108" t="s">
+      <c r="C30" s="110" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="54">
@@ -9942,9 +10084,9 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="111"/>
-      <c r="B31" s="106"/>
-      <c r="C31" s="108"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="110"/>
       <c r="D31" s="54">
         <v>2010</v>
       </c>
@@ -10010,9 +10152,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="111"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="108"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="110"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -10078,11 +10220,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="111"/>
-      <c r="B33" s="105">
+      <c r="A33" s="113"/>
+      <c r="B33" s="107">
         <v>11</v>
       </c>
-      <c r="C33" s="108" t="s">
+      <c r="C33" s="110" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="54">
@@ -10150,9 +10292,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="111"/>
-      <c r="B34" s="106"/>
-      <c r="C34" s="108"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="110"/>
       <c r="D34" s="54">
         <v>2010</v>
       </c>
@@ -10218,9 +10360,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="111"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="110"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -10286,11 +10428,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="111"/>
-      <c r="B36" s="105">
+      <c r="A36" s="113"/>
+      <c r="B36" s="107">
         <v>12</v>
       </c>
-      <c r="C36" s="108" t="s">
+      <c r="C36" s="110" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="54">
@@ -10358,9 +10500,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="111"/>
-      <c r="B37" s="106"/>
-      <c r="C37" s="108"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="110"/>
       <c r="D37" s="54">
         <v>2010</v>
       </c>
@@ -10426,9 +10568,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="111"/>
-      <c r="B38" s="107"/>
-      <c r="C38" s="108"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="110"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -10494,11 +10636,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="111"/>
-      <c r="B39" s="105">
+      <c r="A39" s="113"/>
+      <c r="B39" s="107">
         <v>13</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="110" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="54">
@@ -10566,9 +10708,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="111"/>
-      <c r="B40" s="106"/>
-      <c r="C40" s="108"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="110"/>
       <c r="D40" s="54">
         <v>2010</v>
       </c>
@@ -10634,9 +10776,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="111"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="108"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="110"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -10702,79 +10844,79 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="111"/>
+      <c r="A42" s="113"/>
     </row>
     <row r="43" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="111"/>
+      <c r="A43" s="113"/>
       <c r="B43" s="73"/>
-      <c r="C43" s="120" t="s">
+      <c r="C43" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="120" t="s">
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="120" t="s">
+      <c r="G43" s="122"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="120"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120" t="s">
+      <c r="J43" s="122"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
-      <c r="O43" s="120" t="s">
+      <c r="M43" s="122"/>
+      <c r="N43" s="122"/>
+      <c r="O43" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="120"/>
-      <c r="Q43" s="120"/>
-      <c r="R43" s="117" t="s">
+      <c r="P43" s="122"/>
+      <c r="Q43" s="122"/>
+      <c r="R43" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="S43" s="118"/>
-      <c r="T43" s="119"/>
-      <c r="U43" s="120" t="s">
+      <c r="S43" s="120"/>
+      <c r="T43" s="121"/>
+      <c r="U43" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="V43" s="120"/>
-      <c r="W43" s="120"/>
-      <c r="X43" s="117" t="s">
+      <c r="V43" s="122"/>
+      <c r="W43" s="122"/>
+      <c r="X43" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="118"/>
-      <c r="Z43" s="119"/>
-      <c r="AA43" s="120" t="s">
+      <c r="Y43" s="120"/>
+      <c r="Z43" s="121"/>
+      <c r="AA43" s="122" t="s">
         <v>105</v>
       </c>
-      <c r="AB43" s="120"/>
-      <c r="AC43" s="120"/>
-      <c r="AD43" s="120" t="s">
+      <c r="AB43" s="122"/>
+      <c r="AC43" s="122"/>
+      <c r="AD43" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="AE43" s="120"/>
-      <c r="AF43" s="120"/>
-      <c r="AG43" s="120" t="s">
+      <c r="AE43" s="122"/>
+      <c r="AF43" s="122"/>
+      <c r="AG43" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="AH43" s="120"/>
-      <c r="AI43" s="120"/>
-      <c r="AJ43" s="120" t="s">
+      <c r="AH43" s="122"/>
+      <c r="AI43" s="122"/>
+      <c r="AJ43" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="AK43" s="120"/>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="120" t="s">
+      <c r="AK43" s="122"/>
+      <c r="AL43" s="122"/>
+      <c r="AM43" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="AN43" s="120"/>
-      <c r="AO43" s="120"/>
+      <c r="AN43" s="122"/>
+      <c r="AO43" s="122"/>
     </row>
     <row r="44" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A44" s="112"/>
+      <c r="A44" s="114"/>
       <c r="B44" s="73"/>
       <c r="C44" s="73" t="s">
         <v>72</v>
@@ -11015,10 +11157,10 @@
       </c>
     </row>
     <row r="46" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="121" t="s">
+      <c r="A46" s="123" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="122"/>
+      <c r="B46" s="124"/>
       <c r="C46" s="79">
         <v>2006</v>
       </c>
@@ -11055,10 +11197,10 @@
       <c r="Y46" s="100"/>
     </row>
     <row r="47" spans="1:41" ht="16" thickTop="1">
-      <c r="A47" s="123" t="s">
+      <c r="A47" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="123"/>
+      <c r="B47" s="125"/>
       <c r="C47">
         <f xml:space="preserve"> C45/115</f>
         <v>3.4782608695652174E-2</v>
@@ -11217,10 +11359,10 @@
       </c>
     </row>
     <row r="48" spans="1:41">
-      <c r="A48" s="124" t="s">
+      <c r="A48" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="124"/>
+      <c r="B48" s="126"/>
       <c r="C48">
         <f xml:space="preserve"> C47*72</f>
         <v>2.5043478260869567</v>
@@ -11379,10 +11521,10 @@
       </c>
     </row>
     <row r="49" spans="1:41" s="80" customFormat="1">
-      <c r="A49" s="125" t="s">
+      <c r="A49" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="125"/>
+      <c r="B49" s="127"/>
       <c r="C49" s="80">
         <f xml:space="preserve"> 72-C48</f>
         <v>69.495652173913044</v>
@@ -11692,77 +11834,77 @@
       <c r="X54" s="85"/>
     </row>
     <row r="55" spans="1:41">
-      <c r="C55" s="120" t="s">
+      <c r="C55" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="120"/>
-      <c r="E55" s="120"/>
-      <c r="F55" s="117" t="s">
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="118"/>
-      <c r="H55" s="119"/>
-      <c r="I55" s="120" t="s">
+      <c r="G55" s="120"/>
+      <c r="H55" s="121"/>
+      <c r="I55" s="122" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="120"/>
-      <c r="K55" s="120"/>
-      <c r="L55" s="120" t="s">
+      <c r="J55" s="122"/>
+      <c r="K55" s="122"/>
+      <c r="L55" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="120"/>
-      <c r="N55" s="120"/>
-      <c r="O55" s="120" t="s">
+      <c r="M55" s="122"/>
+      <c r="N55" s="122"/>
+      <c r="O55" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="P55" s="120"/>
-      <c r="Q55" s="120"/>
-      <c r="R55" s="117" t="s">
+      <c r="P55" s="122"/>
+      <c r="Q55" s="122"/>
+      <c r="R55" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="118"/>
-      <c r="T55" s="119"/>
-      <c r="U55" s="120" t="s">
+      <c r="S55" s="120"/>
+      <c r="T55" s="121"/>
+      <c r="U55" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="V55" s="120"/>
-      <c r="W55" s="120"/>
-      <c r="X55" s="120" t="s">
+      <c r="V55" s="122"/>
+      <c r="W55" s="122"/>
+      <c r="X55" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="Y55" s="120"/>
-      <c r="Z55" s="120"/>
-      <c r="AA55" s="120" t="s">
+      <c r="Y55" s="122"/>
+      <c r="Z55" s="122"/>
+      <c r="AA55" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="AB55" s="120"/>
-      <c r="AC55" s="120"/>
-      <c r="AD55" s="120" t="s">
+      <c r="AB55" s="122"/>
+      <c r="AC55" s="122"/>
+      <c r="AD55" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="120"/>
-      <c r="AF55" s="120"/>
-      <c r="AG55" s="120" t="s">
+      <c r="AE55" s="122"/>
+      <c r="AF55" s="122"/>
+      <c r="AG55" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="120"/>
-      <c r="AI55" s="120"/>
-      <c r="AJ55" s="120" t="s">
+      <c r="AH55" s="122"/>
+      <c r="AI55" s="122"/>
+      <c r="AJ55" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="120"/>
-      <c r="AL55" s="120"/>
-      <c r="AM55" s="120" t="s">
+      <c r="AK55" s="122"/>
+      <c r="AL55" s="122"/>
+      <c r="AM55" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="AN55" s="120"/>
-      <c r="AO55" s="120"/>
+      <c r="AN55" s="122"/>
+      <c r="AO55" s="122"/>
     </row>
     <row r="56" spans="1:41" ht="70">
-      <c r="A56" s="126" t="s">
+      <c r="A56" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="127"/>
+      <c r="B56" s="129"/>
       <c r="C56" s="74" t="s">
         <v>99</v>
       </c>
@@ -11882,8 +12024,8 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="16" thickBot="1">
-      <c r="A57" s="128"/>
-      <c r="B57" s="129"/>
+      <c r="A57" s="130"/>
+      <c r="B57" s="131"/>
       <c r="C57" s="74">
         <v>23</v>
       </c>
@@ -12003,10 +12145,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="16" thickTop="1">
-      <c r="A58" s="123" t="s">
+      <c r="A58" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="B58" s="123"/>
+      <c r="B58" s="125"/>
       <c r="C58">
         <f xml:space="preserve"> C57/115</f>
         <v>0.2</v>
@@ -12165,10 +12307,10 @@
       </c>
     </row>
     <row r="59" spans="1:41">
-      <c r="A59" s="124" t="s">
+      <c r="A59" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="124"/>
+      <c r="B59" s="126"/>
       <c r="C59">
         <f xml:space="preserve"> C58*65</f>
         <v>13</v>
@@ -12327,10 +12469,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="125" t="s">
+      <c r="A60" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="125"/>
+      <c r="B60" s="127"/>
       <c r="C60" s="80">
         <f xml:space="preserve"> 65-C59</f>
         <v>52</v>
@@ -12511,9 +12653,6 @@
     <mergeCell ref="I55:K55"/>
     <mergeCell ref="L55:N55"/>
     <mergeCell ref="R55:T55"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
     <mergeCell ref="AM55:AO55"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="AD55:AF55"/>
@@ -12521,34 +12660,37 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="C21:C23"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="AD43:AF43"/>
     <mergeCell ref="AG43:AI43"/>
     <mergeCell ref="AJ43:AL43"/>
     <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="X43:Z43"/>
+    <mergeCell ref="AA43:AC43"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="L43:N43"/>
     <mergeCell ref="O43:Q43"/>
     <mergeCell ref="U43:W43"/>
-    <mergeCell ref="X43:Z43"/>
-    <mergeCell ref="AA43:AC43"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="F43:H43"/>
     <mergeCell ref="I43:K43"/>
     <mergeCell ref="A3:A44"/>
-    <mergeCell ref="X1:X2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
@@ -12556,14 +12698,14 @@
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -12577,60 +12719,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:Y23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="46"/>
     <col min="3" max="3" width="13.5" style="46" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="46"/>
+    <col min="4" max="22" width="8.83203125" style="46"/>
+    <col min="26" max="16384" width="8.83203125" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-    </row>
-    <row r="2" spans="1:19" ht="84">
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+    </row>
+    <row r="2" spans="1:25" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -12673,9 +12816,18 @@
       <c r="S2" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="W2" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A3" s="112" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -12732,9 +12884,18 @@
       <c r="S3" s="8">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="111"/>
+      <c r="W3">
+        <v>2006</v>
+      </c>
+      <c r="X3">
+        <v>0.87</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="113"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -12789,9 +12950,18 @@
       <c r="S4" s="8">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="111"/>
+      <c r="W4">
+        <v>2010</v>
+      </c>
+      <c r="X4" s="104">
+        <v>0.9</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A5" s="113"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -12846,9 +13016,18 @@
       <c r="S5" s="5">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="111"/>
+      <c r="W5">
+        <v>2014</v>
+      </c>
+      <c r="X5" s="26">
+        <v>0.95</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="113"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -12903,9 +13082,18 @@
       <c r="S6" s="7">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="111"/>
+      <c r="W6">
+        <v>2006</v>
+      </c>
+      <c r="X6">
+        <v>0.66</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A7" s="113"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -12960,9 +13148,18 @@
       <c r="S7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="111"/>
+      <c r="W7">
+        <v>2010</v>
+      </c>
+      <c r="X7" s="104">
+        <v>0.71</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A8" s="113"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -13017,9 +13214,18 @@
       <c r="S8" s="8">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="111"/>
+      <c r="W8">
+        <v>2014</v>
+      </c>
+      <c r="X8" s="26">
+        <v>0.74</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A9" s="113"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -13074,9 +13280,18 @@
       <c r="S9" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="111"/>
+      <c r="W9">
+        <v>2006</v>
+      </c>
+      <c r="X9">
+        <v>0.69</v>
+      </c>
+      <c r="Y9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="113"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -13131,9 +13346,18 @@
       <c r="S10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="111"/>
+      <c r="W10">
+        <v>2010</v>
+      </c>
+      <c r="X10" s="104">
+        <v>0.69</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="113"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -13188,9 +13412,18 @@
       <c r="S11" s="8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="111"/>
+      <c r="W11">
+        <v>2014</v>
+      </c>
+      <c r="X11" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="113"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -13245,9 +13478,18 @@
       <c r="S12" s="8">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="111"/>
+      <c r="W12">
+        <v>2006</v>
+      </c>
+      <c r="X12">
+        <v>0.41</v>
+      </c>
+      <c r="Y12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="113"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -13302,9 +13544,18 @@
       <c r="S13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="111"/>
+      <c r="W13">
+        <v>2010</v>
+      </c>
+      <c r="X13" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="Y13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="113"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -13359,9 +13610,18 @@
       <c r="S14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="111"/>
+      <c r="W14">
+        <v>2014</v>
+      </c>
+      <c r="X14" s="26">
+        <v>0.67</v>
+      </c>
+      <c r="Y14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="113"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -13416,8 +13676,17 @@
       <c r="S15" s="5">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="W15">
+        <v>2006</v>
+      </c>
+      <c r="X15">
+        <v>1.22</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="B16" s="45" t="s">
         <v>69</v>
       </c>
@@ -13472,8 +13741,28 @@
       <c r="S16" s="46">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="W16">
+        <v>2010</v>
+      </c>
+      <c r="X16" s="104">
+        <v>1.28</v>
+      </c>
+      <c r="Y16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="W17">
+        <v>2014</v>
+      </c>
+      <c r="X17" s="26">
+        <v>1.36</v>
+      </c>
+      <c r="Y17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" s="47" t="s">
         <v>68</v>
       </c>
@@ -13519,8 +13808,17 @@
       <c r="O18" s="8">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="W18">
+        <v>2006</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="45" t="s">
         <v>55</v>
       </c>
@@ -13566,8 +13864,17 @@
       <c r="O19" s="8">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="W19">
+        <v>2010</v>
+      </c>
+      <c r="X19" s="105">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="45" t="s">
         <v>57</v>
       </c>
@@ -13613,8 +13920,17 @@
       <c r="O20" s="5">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="W20">
+        <v>2014</v>
+      </c>
+      <c r="X20" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="45" t="s">
         <v>58</v>
       </c>
@@ -13660,8 +13976,17 @@
       <c r="O21" s="7">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="W21">
+        <v>2006</v>
+      </c>
+      <c r="X21">
+        <v>0.98</v>
+      </c>
+      <c r="Y21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="45" t="s">
         <v>59</v>
       </c>
@@ -13707,8 +14032,17 @@
       <c r="O22" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="W22">
+        <v>2010</v>
+      </c>
+      <c r="X22" s="105">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="45" t="s">
         <v>60</v>
       </c>
@@ -13754,8 +14088,17 @@
       <c r="O23" s="8">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="W23">
+        <v>2014</v>
+      </c>
+      <c r="X23" s="27">
+        <v>1.01</v>
+      </c>
+      <c r="Y23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" s="45" t="s">
         <v>61</v>
       </c>
@@ -13802,7 +14145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:26">
       <c r="A25" s="45" t="s">
         <v>62</v>
       </c>
@@ -13849,7 +14192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:26">
       <c r="A26" s="45" t="s">
         <v>56</v>
       </c>
@@ -13896,7 +14239,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:26">
       <c r="A27" s="45" t="s">
         <v>63</v>
       </c>
@@ -13943,7 +14286,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:26">
       <c r="A28" s="45" t="s">
         <v>64</v>
       </c>
@@ -13990,7 +14333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:26" ht="14">
       <c r="A29" s="45" t="s">
         <v>65</v>
       </c>
@@ -14036,8 +14379,29 @@
       <c r="O29" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="T29" s="104">
+        <v>0.9</v>
+      </c>
+      <c r="U29" s="104">
+        <v>0.71</v>
+      </c>
+      <c r="V29" s="104">
+        <v>0.69</v>
+      </c>
+      <c r="W29" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="X29" s="104">
+        <v>1.28</v>
+      </c>
+      <c r="Y29" s="105">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="14">
       <c r="A30" s="45" t="s">
         <v>66</v>
       </c>
@@ -14082,6 +14446,27 @@
       </c>
       <c r="O30" s="5">
         <v>0.43</v>
+      </c>
+      <c r="T30" s="26">
+        <v>0.95</v>
+      </c>
+      <c r="U30" s="26">
+        <v>0.74</v>
+      </c>
+      <c r="V30" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="W30" s="26">
+        <v>0.67</v>
+      </c>
+      <c r="X30" s="26">
+        <v>1.36</v>
+      </c>
+      <c r="Y30" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="27">
+        <v>1.01</v>
       </c>
     </row>
   </sheetData>
@@ -14096,6 +14481,7 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14123,44 +14509,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -14205,7 +14591,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -14264,7 +14650,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="111"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -14321,7 +14707,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A5" s="111"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -14378,7 +14764,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="111"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -14435,7 +14821,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A7" s="111"/>
+      <c r="A7" s="113"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -14492,7 +14878,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="111"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -14549,7 +14935,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A9" s="111"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -14606,7 +14992,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="111"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -14663,7 +15049,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="111"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -14720,7 +15106,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="111"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -14777,7 +15163,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="111"/>
+      <c r="A13" s="113"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -14834,7 +15220,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="111"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -14891,7 +15277,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="111"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -15705,44 +16091,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -15787,7 +16173,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -15846,7 +16232,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="111"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -15903,7 +16289,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="24">
-      <c r="A5" s="111"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -15960,7 +16346,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="111"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -16017,7 +16403,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
-      <c r="A7" s="111"/>
+      <c r="A7" s="113"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -16074,7 +16460,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="111"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -16131,7 +16517,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
-      <c r="A9" s="111"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -16188,7 +16574,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="111"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -16245,7 +16631,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="111"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -16302,7 +16688,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="111"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -16359,7 +16745,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="111"/>
+      <c r="A13" s="113"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -16416,7 +16802,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="111"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -16473,7 +16859,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="111"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -16594,171 +16980,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="20" customHeight="1">
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
     </row>
     <row r="2" spans="1:44" ht="20" customHeight="1">
-      <c r="C2" s="105">
-        <v>1</v>
-      </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="105">
+      <c r="C2" s="107">
+        <v>1</v>
+      </c>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="107">
         <v>2</v>
       </c>
-      <c r="G2" s="106"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="105">
+      <c r="G2" s="108"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="107">
         <v>3</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="105">
+      <c r="J2" s="108"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="107">
         <v>4</v>
       </c>
-      <c r="M2" s="106"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="105">
+      <c r="M2" s="108"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="107">
         <v>5</v>
       </c>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="105">
+      <c r="P2" s="108"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="107">
         <v>6</v>
       </c>
-      <c r="S2" s="106"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="105">
+      <c r="S2" s="108"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="107">
         <v>7</v>
       </c>
-      <c r="V2" s="106"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="105">
+      <c r="V2" s="108"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="107">
         <v>8</v>
       </c>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="105">
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="107">
         <v>14</v>
       </c>
-      <c r="AB2" s="106"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="105">
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="109"/>
+      <c r="AD2" s="107">
         <v>9</v>
       </c>
-      <c r="AE2" s="106"/>
-      <c r="AF2" s="107"/>
-      <c r="AG2" s="105">
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="109"/>
+      <c r="AG2" s="107">
         <v>10</v>
       </c>
-      <c r="AH2" s="106"/>
-      <c r="AI2" s="107"/>
-      <c r="AJ2" s="105">
+      <c r="AH2" s="108"/>
+      <c r="AI2" s="109"/>
+      <c r="AJ2" s="107">
         <v>11</v>
       </c>
-      <c r="AK2" s="106"/>
-      <c r="AL2" s="107"/>
-      <c r="AM2" s="105">
+      <c r="AK2" s="108"/>
+      <c r="AL2" s="109"/>
+      <c r="AM2" s="107">
         <v>12</v>
       </c>
-      <c r="AN2" s="106"/>
-      <c r="AO2" s="107"/>
-      <c r="AP2" s="105">
+      <c r="AN2" s="108"/>
+      <c r="AO2" s="109"/>
+      <c r="AP2" s="107">
         <v>13</v>
       </c>
-      <c r="AQ2" s="106"/>
-      <c r="AR2" s="107"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="109"/>
     </row>
     <row r="3" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108" t="s">
+      <c r="B3" s="110"/>
+      <c r="C3" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108" t="s">
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108" t="s">
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108" t="s">
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108" t="s">
+      <c r="M3" s="110"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108" t="s">
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108" t="s">
+      <c r="S3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108" t="s">
+      <c r="V3" s="110"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="114" t="s">
+      <c r="Y3" s="110"/>
+      <c r="Z3" s="110"/>
+      <c r="AA3" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="115"/>
-      <c r="AC3" s="116"/>
-      <c r="AD3" s="108" t="s">
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108"/>
-      <c r="AG3" s="108" t="s">
+      <c r="AE3" s="110"/>
+      <c r="AF3" s="110"/>
+      <c r="AG3" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="108"/>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108" t="s">
+      <c r="AH3" s="110"/>
+      <c r="AI3" s="110"/>
+      <c r="AJ3" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108"/>
-      <c r="AM3" s="108" t="s">
+      <c r="AK3" s="110"/>
+      <c r="AL3" s="110"/>
+      <c r="AM3" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="108"/>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108" t="s">
+      <c r="AN3" s="110"/>
+      <c r="AO3" s="110"/>
+      <c r="AP3" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108"/>
+      <c r="AQ3" s="110"/>
+      <c r="AR3" s="110"/>
     </row>
     <row r="4" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="108"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="14">
         <v>2006</v>
       </c>
@@ -16887,10 +17273,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="108"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -17019,7 +17405,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="115" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -17153,7 +17539,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="113"/>
+      <c r="A7" s="115"/>
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
@@ -17285,7 +17671,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="113"/>
+      <c r="A8" s="115"/>
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
@@ -17417,7 +17803,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="113"/>
+      <c r="A9" s="115"/>
       <c r="B9" s="15" t="s">
         <v>51</v>
       </c>
@@ -17549,7 +17935,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="113"/>
+      <c r="A10" s="115"/>
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
@@ -17681,7 +18067,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" ht="20" customHeight="1">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="111" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -17815,7 +18201,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" ht="20" customHeight="1">
-      <c r="A12" s="109"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -17947,7 +18333,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="20" customHeight="1">
-      <c r="A13" s="109"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -18079,7 +18465,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" ht="20" customHeight="1">
-      <c r="A14" s="109"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -18211,7 +18597,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="106" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -18345,7 +18731,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="104"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
@@ -18477,7 +18863,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="20" customHeight="1">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="111" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -18611,7 +18997,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="20" customHeight="1">
-      <c r="A18" s="109"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
@@ -18743,7 +19129,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="20" customHeight="1">
-      <c r="A19" s="109"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
@@ -19648,44 +20034,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="109" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109" t="s">
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -19730,13 +20116,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="105">
-        <v>1</v>
-      </c>
-      <c r="C3" s="108" t="s">
+      <c r="B3" s="107">
+        <v>1</v>
+      </c>
+      <c r="C3" s="110" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="14">
@@ -19789,9 +20175,9 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="111"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="108"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="110"/>
       <c r="D4" s="14">
         <v>2010</v>
       </c>
@@ -19842,9 +20228,9 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="111"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="110"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -19895,11 +20281,11 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="111"/>
-      <c r="B6" s="105">
+      <c r="A6" s="113"/>
+      <c r="B6" s="107">
         <v>2</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="110" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="14">
@@ -19952,9 +20338,9 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="111"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="108"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="110"/>
       <c r="D7" s="14">
         <v>2010</v>
       </c>
@@ -20005,9 +20391,9 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="111"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -20058,11 +20444,11 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="111"/>
-      <c r="B9" s="105">
+      <c r="A9" s="113"/>
+      <c r="B9" s="107">
         <v>3</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="110" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14">
@@ -20115,9 +20501,9 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="111"/>
-      <c r="B10" s="106"/>
-      <c r="C10" s="108"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="110"/>
       <c r="D10" s="14">
         <v>2010</v>
       </c>
@@ -20168,9 +20554,9 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="111"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="108"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -20221,11 +20607,11 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="111"/>
-      <c r="B12" s="105">
+      <c r="A12" s="113"/>
+      <c r="B12" s="107">
         <v>4</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="110" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14">
@@ -20278,9 +20664,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="111"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="108"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="14">
         <v>2010</v>
       </c>
@@ -20331,9 +20717,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="111"/>
-      <c r="B14" s="107"/>
-      <c r="C14" s="108"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -20384,11 +20770,11 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="111"/>
-      <c r="B15" s="105">
+      <c r="A15" s="113"/>
+      <c r="B15" s="107">
         <v>5</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="110" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="14">
@@ -20441,9 +20827,9 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="111"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="108"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="110"/>
       <c r="D16" s="14">
         <v>2010</v>
       </c>
@@ -20494,9 +20880,9 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="111"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -20547,11 +20933,11 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="111"/>
-      <c r="B18" s="105">
+      <c r="A18" s="113"/>
+      <c r="B18" s="107">
         <v>6</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="110" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="14">
@@ -20604,9 +20990,9 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="111"/>
-      <c r="B19" s="106"/>
-      <c r="C19" s="108"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="14">
         <v>2010</v>
       </c>
@@ -20657,9 +21043,9 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="111"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="108"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -20710,11 +21096,11 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="111"/>
-      <c r="B21" s="105">
+      <c r="A21" s="113"/>
+      <c r="B21" s="107">
         <v>7</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="110" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="14">
@@ -20767,9 +21153,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="111"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="108"/>
+      <c r="A22" s="113"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="110"/>
       <c r="D22" s="14">
         <v>2010</v>
       </c>
@@ -20820,9 +21206,9 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="111"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
+      <c r="A23" s="113"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -20873,11 +21259,11 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="111"/>
-      <c r="B24" s="105">
+      <c r="A24" s="113"/>
+      <c r="B24" s="107">
         <v>8</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="110" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14">
@@ -20930,9 +21316,9 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="111"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="108"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="110"/>
       <c r="D25" s="14">
         <v>2010</v>
       </c>
@@ -20983,9 +21369,9 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="111"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="108"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="110"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -21036,11 +21422,11 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="111"/>
-      <c r="B27" s="105">
+      <c r="A27" s="113"/>
+      <c r="B27" s="107">
         <v>14</v>
       </c>
-      <c r="C27" s="114" t="s">
+      <c r="C27" s="116" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="14">
@@ -21093,9 +21479,9 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="111"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="115"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="117"/>
       <c r="D28" s="14">
         <v>2010</v>
       </c>
@@ -21146,9 +21532,9 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="111"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="116"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -21199,11 +21585,11 @@
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="111"/>
-      <c r="B30" s="105">
+      <c r="A30" s="113"/>
+      <c r="B30" s="107">
         <v>9</v>
       </c>
-      <c r="C30" s="108" t="s">
+      <c r="C30" s="110" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="14">
@@ -21256,9 +21642,9 @@
       </c>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="111"/>
-      <c r="B31" s="106"/>
-      <c r="C31" s="108"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="110"/>
       <c r="D31" s="14">
         <v>2010</v>
       </c>
@@ -21309,9 +21695,9 @@
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="111"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="108"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="110"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -21362,11 +21748,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="111"/>
-      <c r="B33" s="105">
+      <c r="A33" s="113"/>
+      <c r="B33" s="107">
         <v>10</v>
       </c>
-      <c r="C33" s="108" t="s">
+      <c r="C33" s="110" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="14">
@@ -21419,9 +21805,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="111"/>
-      <c r="B34" s="106"/>
-      <c r="C34" s="108"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="110"/>
       <c r="D34" s="14">
         <v>2010</v>
       </c>
@@ -21472,9 +21858,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="111"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="110"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -21525,11 +21911,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="111"/>
-      <c r="B36" s="105">
+      <c r="A36" s="113"/>
+      <c r="B36" s="107">
         <v>11</v>
       </c>
-      <c r="C36" s="108" t="s">
+      <c r="C36" s="110" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="14">
@@ -21582,9 +21968,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="111"/>
-      <c r="B37" s="106"/>
-      <c r="C37" s="108"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="110"/>
       <c r="D37" s="14">
         <v>2010</v>
       </c>
@@ -21635,9 +22021,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="111"/>
-      <c r="B38" s="107"/>
-      <c r="C38" s="108"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="110"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -21688,11 +22074,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="111"/>
-      <c r="B39" s="105">
+      <c r="A39" s="113"/>
+      <c r="B39" s="107">
         <v>12</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="110" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14">
@@ -21745,9 +22131,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="111"/>
-      <c r="B40" s="106"/>
-      <c r="C40" s="108"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="110"/>
       <c r="D40" s="14">
         <v>2010</v>
       </c>
@@ -21798,9 +22184,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="111"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="108"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="110"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -21851,11 +22237,11 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="111"/>
-      <c r="B42" s="105">
+      <c r="A42" s="113"/>
+      <c r="B42" s="107">
         <v>13</v>
       </c>
-      <c r="C42" s="108" t="s">
+      <c r="C42" s="110" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="14">
@@ -21908,9 +22294,9 @@
       </c>
     </row>
     <row r="43" spans="1:41">
-      <c r="A43" s="111"/>
-      <c r="B43" s="106"/>
-      <c r="C43" s="108"/>
+      <c r="A43" s="113"/>
+      <c r="B43" s="108"/>
+      <c r="C43" s="110"/>
       <c r="D43" s="14">
         <v>2010</v>
       </c>
@@ -21961,9 +22347,9 @@
       </c>
     </row>
     <row r="44" spans="1:41">
-      <c r="A44" s="112"/>
-      <c r="B44" s="107"/>
-      <c r="C44" s="108"/>
+      <c r="A44" s="114"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="110"/>
       <c r="D44" s="25">
         <v>2014</v>
       </c>
@@ -22014,81 +22400,81 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A46" s="108" t="s">
+      <c r="A46" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="108"/>
-      <c r="C46" s="108" t="s">
+      <c r="B46" s="110"/>
+      <c r="C46" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="108"/>
-      <c r="E46" s="108"/>
-      <c r="F46" s="108" t="s">
+      <c r="D46" s="110"/>
+      <c r="E46" s="110"/>
+      <c r="F46" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="108"/>
-      <c r="H46" s="108"/>
-      <c r="I46" s="108" t="s">
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
+      <c r="I46" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="108"/>
-      <c r="K46" s="108"/>
-      <c r="L46" s="108" t="s">
+      <c r="J46" s="110"/>
+      <c r="K46" s="110"/>
+      <c r="L46" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="108"/>
-      <c r="N46" s="108"/>
-      <c r="O46" s="108" t="s">
+      <c r="M46" s="110"/>
+      <c r="N46" s="110"/>
+      <c r="O46" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="P46" s="108"/>
-      <c r="Q46" s="108"/>
-      <c r="R46" s="108" t="s">
+      <c r="P46" s="110"/>
+      <c r="Q46" s="110"/>
+      <c r="R46" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="S46" s="108"/>
-      <c r="T46" s="108"/>
-      <c r="U46" s="114" t="s">
+      <c r="S46" s="110"/>
+      <c r="T46" s="110"/>
+      <c r="U46" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="115"/>
-      <c r="W46" s="116"/>
-      <c r="X46" s="114" t="s">
+      <c r="V46" s="117"/>
+      <c r="W46" s="118"/>
+      <c r="X46" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="115"/>
-      <c r="Z46" s="116"/>
-      <c r="AA46" s="108" t="s">
+      <c r="Y46" s="117"/>
+      <c r="Z46" s="118"/>
+      <c r="AA46" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="AB46" s="108"/>
-      <c r="AC46" s="108"/>
-      <c r="AD46" s="108" t="s">
+      <c r="AB46" s="110"/>
+      <c r="AC46" s="110"/>
+      <c r="AD46" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="AE46" s="108"/>
-      <c r="AF46" s="108"/>
-      <c r="AG46" s="108" t="s">
+      <c r="AE46" s="110"/>
+      <c r="AF46" s="110"/>
+      <c r="AG46" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="108"/>
-      <c r="AI46" s="108"/>
-      <c r="AJ46" s="108" t="s">
+      <c r="AH46" s="110"/>
+      <c r="AI46" s="110"/>
+      <c r="AJ46" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="AK46" s="108"/>
-      <c r="AL46" s="108"/>
-      <c r="AM46" s="108" t="s">
+      <c r="AK46" s="110"/>
+      <c r="AL46" s="110"/>
+      <c r="AM46" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="AN46" s="108"/>
-      <c r="AO46" s="108"/>
+      <c r="AN46" s="110"/>
+      <c r="AO46" s="110"/>
     </row>
     <row r="47" spans="1:41" ht="42.75" customHeight="1">
-      <c r="A47" s="108" t="s">
+      <c r="A47" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="108"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="54" t="s">
         <v>72</v>
       </c>
@@ -22208,10 +22594,10 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="33" customHeight="1">
-      <c r="A48" s="108" t="s">
+      <c r="A48" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="108"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="54">
         <v>4</v>
       </c>
@@ -22331,7 +22717,7 @@
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="131" t="s">
+      <c r="B49" s="133" t="s">
         <v>91</v>
       </c>
       <c r="C49" s="63">
@@ -22342,7 +22728,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="124"/>
+      <c r="B50" s="126"/>
       <c r="C50" s="63">
         <v>2010</v>
       </c>
@@ -22351,7 +22737,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="124"/>
+      <c r="B51" s="126"/>
       <c r="C51" s="63">
         <v>2014</v>
       </c>

</xml_diff>